<commit_message>
attendance from first meeting
</commit_message>
<xml_diff>
--- a/meeting_attendance.xlsx
+++ b/meeting_attendance.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julietwield/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julietwield/Desktop/julietwield-project3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5211B4AB-21D9-9F4E-802A-57D5BD8B1AB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFEFD4C0-887B-0045-9601-5D492070DC9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="15840" windowHeight="21600" xr2:uid="{7B038190-2AF9-6F4E-B15F-676D94CBC681}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="15840" windowHeight="19780" xr2:uid="{7B038190-2AF9-6F4E-B15F-676D94CBC681}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Attendance</t>
   </si>
@@ -47,6 +46,9 @@
   </si>
   <si>
     <t>Time</t>
+  </si>
+  <si>
+    <t>all attended</t>
   </si>
 </sst>
 </file>
@@ -403,7 +405,7 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -431,6 +433,9 @@
       <c r="B2" s="2">
         <v>0.20833333333333334</v>
       </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1">

</xml_diff>